<commit_message>
update status for no pr or invoice found
</commit_message>
<xml_diff>
--- a/BaswareAutomation/Output/OutputDataProvide.xlsx
+++ b/BaswareAutomation/Output/OutputDataProvide.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -324,12 +324,22 @@
   </si>
   <si>
     <t>EMEAAD\laroche</t>
+  </si>
+  <si>
+    <t>Test Status</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -384,12 +394,32 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -420,7 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -437,6 +467,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -718,7 +752,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF5"/>
+  <dimension ref="A1:AH5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -726,33 +760,33 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.140625" customWidth="1"/>
-    <col min="17" max="17" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.5703125" customWidth="1"/>
-    <col min="19" max="19" width="26" customWidth="1"/>
-    <col min="20" max="20" width="21.85546875" customWidth="1"/>
-    <col min="21" max="21" width="16.140625" customWidth="1"/>
-    <col min="22" max="22" width="7.42578125" customWidth="1"/>
-    <col min="23" max="24" width="15.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="19.7109375" customWidth="1"/>
-    <col min="30" max="30" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="39.28515625" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="11.85546875" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="32.28515625" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.140625" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="13.7109375" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="29.85546875" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="40.7109375" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.85546875" collapsed="false"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="8.7109375" collapsed="false"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.42578125" collapsed="false"/>
+    <col min="16" max="16" customWidth="true" width="17.140625" collapsed="false"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="22.5703125" collapsed="false"/>
+    <col min="18" max="18" customWidth="true" width="23.5703125" collapsed="false"/>
+    <col min="19" max="19" customWidth="true" width="26.0" collapsed="false"/>
+    <col min="20" max="20" customWidth="true" width="21.85546875" collapsed="false"/>
+    <col min="21" max="21" customWidth="true" width="16.140625" collapsed="false"/>
+    <col min="22" max="22" customWidth="true" width="7.42578125" collapsed="false"/>
+    <col min="23" max="24" customWidth="true" style="1" width="15.85546875" collapsed="false"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="27" max="29" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="23.140625" collapsed="false"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="16.85546875" collapsed="false"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="17.5703125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -852,6 +886,9 @@
       <c r="AF1" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="AH1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="2" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -950,6 +987,9 @@
       <c r="AF2" s="11" t="s">
         <v>40</v>
       </c>
+      <c r="AH2" t="s" s="12">
+        <v>88</v>
+      </c>
     </row>
     <row r="3" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1048,6 +1088,9 @@
       <c r="AF3" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="AH3" t="s" s="13">
+        <v>88</v>
+      </c>
     </row>
     <row r="4" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1144,6 +1187,9 @@
       <c r="AF4" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="AH4" t="s" s="14">
+        <v>89</v>
+      </c>
     </row>
     <row r="5" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1241,6 +1287,9 @@
       </c>
       <c r="AF5" s="2" t="s">
         <v>38</v>
+      </c>
+      <c r="AH5" t="s" s="15">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Demo Data to Teams
</commit_message>
<xml_diff>
--- a/BaswareAutomation/Output/OutputDataProvide.xlsx
+++ b/BaswareAutomation/Output/OutputDataProvide.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -179,9 +179,6 @@
     <t>STANDARD</t>
   </si>
   <si>
-    <t>EMEAAD\proch</t>
-  </si>
-  <si>
     <t>Approver3</t>
   </si>
   <si>
@@ -212,15 +209,9 @@
     <t>10</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>300</t>
   </si>
   <si>
-    <t>1000</t>
-  </si>
-  <si>
     <t>Aix  Golf</t>
   </si>
   <si>
@@ -236,9 +227,6 @@
     <t>Purchase requisition</t>
   </si>
   <si>
-    <t>146</t>
-  </si>
-  <si>
     <t>136</t>
   </si>
   <si>
@@ -248,39 +236,15 @@
     <t>TEST_AUTO_OAR_08032022_01</t>
   </si>
   <si>
-    <t>TEST_AUTO_OAR_08032022_02</t>
-  </si>
-  <si>
     <t>TEST_AUTO_OAR_08032022_03</t>
   </si>
   <si>
-    <t>TEST_AUTO_OAR_08032022_04</t>
-  </si>
-  <si>
-    <t>Product2</t>
-  </si>
-  <si>
     <t>Product3</t>
   </si>
   <si>
-    <t>Product4</t>
-  </si>
-  <si>
-    <t>LOGISTICS</t>
-  </si>
-  <si>
-    <t>BUILDINGS MAINTENANCE</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
-    <t>Logistic</t>
-  </si>
-  <si>
-    <t>CP-AAST</t>
-  </si>
-  <si>
     <t>4290</t>
   </si>
   <si>
@@ -290,27 +254,9 @@
     <t>S00007077001</t>
   </si>
   <si>
-    <t>S00010321001</t>
-  </si>
-  <si>
     <t>Contractors</t>
   </si>
   <si>
-    <t>173</t>
-  </si>
-  <si>
-    <t>Auditor fees</t>
-  </si>
-  <si>
-    <t>S00010242001</t>
-  </si>
-  <si>
-    <t>4293</t>
-  </si>
-  <si>
-    <t>EMEAAD\dcoisplet</t>
-  </si>
-  <si>
     <t>190000</t>
   </si>
   <si>
@@ -318,12 +264,6 @@
   </si>
   <si>
     <t>EMEAAD\pbuisson</t>
-  </si>
-  <si>
-    <t>185000</t>
-  </si>
-  <si>
-    <t>EMEAAD\laroche</t>
   </si>
   <si>
     <t>Test Status</t>
@@ -450,7 +390,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -468,9 +408,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -752,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH5"/>
+  <dimension ref="A1:AH3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A4" sqref="A4:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,7 +771,7 @@
         <v>10</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>33</v>
@@ -884,10 +822,10 @@
         <v>27</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AH1" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -904,10 +842,10 @@
         <v>21</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>26</v>
@@ -916,25 +854,25 @@
         <v>26</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="O2" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>37</v>
@@ -943,52 +881,52 @@
         <v>36</v>
       </c>
       <c r="R2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>34</v>
       </c>
       <c r="W2" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AB2" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AC2" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AE2" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="AF2" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AH2" t="s" s="12">
-        <v>88</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1005,291 +943,89 @@
         <v>21</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K3" s="6" t="s">
+      <c r="Q3" s="2"/>
+      <c r="R3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="U3" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="V3" s="2" t="s">
         <v>34</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="X3" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="Y3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AB3" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AC3" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AE3" s="6" t="s">
-        <v>40</v>
+        <v>65</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="AF3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AH3" t="s" s="13">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="W4" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="X4" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AF4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH4" t="s" s="14">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T5" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="W5" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="X5" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AE5" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AH5" t="s" s="15">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1297,14 +1033,12 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;1#&amp;"Tahoma"&amp;9&amp;KCF022BC2 - Restricted</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId6"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>